<commit_message>
Report phase 3.1 and 3.2
</commit_message>
<xml_diff>
--- a/P1/data/table_creation.xlsx
+++ b/P1/data/table_creation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="18240" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>REPTree</t>
   </si>
@@ -72,6 +72,48 @@
   </si>
   <si>
     <t>Agent</t>
+  </si>
+  <si>
+    <t>Comparación de predictores</t>
+  </si>
+  <si>
+    <t>Mean absolute error</t>
+  </si>
+  <si>
+    <t>Root mean squared error</t>
+  </si>
+  <si>
+    <t>Correlation coefficient (x100)</t>
+  </si>
+  <si>
+    <t>Relative absolute error (%)</t>
+  </si>
+  <si>
+    <t>Root relative squared error (%)</t>
+  </si>
+  <si>
+    <t>Predict 2 without class</t>
+  </si>
+  <si>
+    <t>Predict 2 with class</t>
+  </si>
+  <si>
+    <t>Predict 5 with class</t>
+  </si>
+  <si>
+    <t>Predict 5 without class</t>
+  </si>
+  <si>
+    <t>M5 predicts 2</t>
+  </si>
+  <si>
+    <t>M5 predicts 5</t>
+  </si>
+  <si>
+    <t>REPTree predicts 2</t>
+  </si>
+  <si>
+    <t>REPTree predicts 5</t>
   </si>
 </sst>
 </file>
@@ -759,11 +801,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2114627648"/>
-        <c:axId val="-2106422160"/>
+        <c:axId val="-2135676608"/>
+        <c:axId val="-2136098160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2114627648"/>
+        <c:axId val="-2135676608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -799,7 +841,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2106422160"/>
+        <c:crossAx val="-2136098160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -807,7 +849,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2106422160"/>
+        <c:axId val="-2136098160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -831,7 +873,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114627648"/>
+        <c:crossAx val="-2135676608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1369,12 +1411,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-2083036160"/>
-        <c:axId val="-2109354832"/>
+        <c:axId val="-2135548384"/>
+        <c:axId val="-2135544944"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-2083036160"/>
+        <c:axId val="-2135548384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1410,7 +1452,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2109354832"/>
+        <c:crossAx val="-2135544944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1418,7 +1460,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2109354832"/>
+        <c:axId val="-2135544944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1468,7 +1510,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2083036160"/>
+        <c:crossAx val="-2135548384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1829,11 +1871,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="-2054118976"/>
-        <c:axId val="-2054093520"/>
+        <c:axId val="-2135503920"/>
+        <c:axId val="-2135500576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2054118976"/>
+        <c:axId val="-2135503920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1875,7 +1917,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2054093520"/>
+        <c:crossAx val="-2135500576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1883,7 +1925,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2054093520"/>
+        <c:axId val="-2135500576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1933,7 +1975,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2054118976"/>
+        <c:crossAx val="-2135503920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1962,6 +2004,1435 @@
         <a:p>
           <a:pPr>
             <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>With our Without Class Comparison</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$107</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Predict 2 with class</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$108:$B$112</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Correlation coefficient (x100)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mean absolute error</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Root mean squared error</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Relative absolute error (%)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Root relative squared error (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$108:$C$112</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>93.23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46.6545</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>79.4473</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.8858</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36.2288</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$107</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Predict 2 without class</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$108:$B$112</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Correlation coefficient (x100)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mean absolute error</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Root mean squared error</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Relative absolute error (%)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Root relative squared error (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$108:$D$112</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>93.23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46.3957</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>79.4306</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.7533</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36.2212</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$107</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Predict 5 with class</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$108:$B$112</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Correlation coefficient (x100)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mean absolute error</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Root mean squared error</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Relative absolute error (%)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Root relative squared error (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$108:$E$112</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>91.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51.1191</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84.7766</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.3991</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39.3311</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$107</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Predict 5 without class</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$108:$B$112</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Correlation coefficient (x100)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mean absolute error</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Root mean squared error</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Relative absolute error (%)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Root relative squared error (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$108:$F$112</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>91.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51.4899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84.7849</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.5978</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39.335</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="118"/>
+        <c:overlap val="-28"/>
+        <c:axId val="-2062597280"/>
+        <c:axId val="-2076334128"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2062597280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2076334128"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2076334128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2062597280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" baseline="0"/>
+              <a:t>Regression accuracy: </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>REPTree vs. M5</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2000"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$144</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>M5 predicts 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$145:$B$149</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Correlation coefficient (x100)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mean absolute error</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Root mean squared error</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Relative absolute error (%)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Root relative squared error (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$145:$C$149</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>94.54</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45.1831</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70.2187</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.2175</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.5772</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$144</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>REPTree predicts 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$145:$B$149</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Correlation coefficient (x100)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mean absolute error</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Root mean squared error</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Relative absolute error (%)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Root relative squared error (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$145:$D$149</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>93.23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46.3957</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>79.4306</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.7533</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36.2212</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$144</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>M5 predicts 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$145:$B$149</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Correlation coefficient (x100)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mean absolute error</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Root mean squared error</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Relative absolute error (%)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Root relative squared error (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$145:$E$149</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>95.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.8079</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>68.1857</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.4284</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31.0934</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$144</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>REPTree predicts 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$145:$B$149</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Correlation coefficient (x100)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mean absolute error</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Root mean squared error</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Relative absolute error (%)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Root relative squared error (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$145:$F$149</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>91.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51.4899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84.7849</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.5978</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39.335</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="-2137803824"/>
+        <c:axId val="-2076738512"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2137803824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2076738512"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2076738512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2137803824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="lt1">
                   <a:lumMod val="85000"/>
@@ -2144,6 +3615,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="294">
   <cs:axisTitle>
@@ -3097,6 +4648,998 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3679,6 +6222,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>179</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3950,15 +6553,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N74"/>
+  <dimension ref="A2:N149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="J72" sqref="J72"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="N158" sqref="N158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
@@ -4596,6 +7199,209 @@
         <v>57.484999999999999</v>
       </c>
     </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B103" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C107" t="s">
+        <v>23</v>
+      </c>
+      <c r="D107" t="s">
+        <v>22</v>
+      </c>
+      <c r="E107" t="s">
+        <v>24</v>
+      </c>
+      <c r="F107" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B108" t="s">
+        <v>19</v>
+      </c>
+      <c r="C108">
+        <v>93.23</v>
+      </c>
+      <c r="D108">
+        <v>93.23</v>
+      </c>
+      <c r="E108">
+        <v>91.95</v>
+      </c>
+      <c r="F108">
+        <v>91.95</v>
+      </c>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B109" t="s">
+        <v>17</v>
+      </c>
+      <c r="C109">
+        <v>46.654499999999999</v>
+      </c>
+      <c r="D109">
+        <v>46.395699999999998</v>
+      </c>
+      <c r="E109">
+        <v>51.119100000000003</v>
+      </c>
+      <c r="F109">
+        <v>51.489899999999999</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B110" t="s">
+        <v>18</v>
+      </c>
+      <c r="C110">
+        <v>79.447299999999998</v>
+      </c>
+      <c r="D110">
+        <v>79.430599999999998</v>
+      </c>
+      <c r="E110">
+        <v>84.776600000000002</v>
+      </c>
+      <c r="F110">
+        <v>84.784899999999993</v>
+      </c>
+    </row>
+    <row r="111" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B111" t="s">
+        <v>20</v>
+      </c>
+      <c r="C111">
+        <v>23.8858</v>
+      </c>
+      <c r="D111">
+        <v>23.753299999999999</v>
+      </c>
+      <c r="E111">
+        <v>27.399100000000001</v>
+      </c>
+      <c r="F111">
+        <v>27.597799999999999</v>
+      </c>
+    </row>
+    <row r="112" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B112" t="s">
+        <v>21</v>
+      </c>
+      <c r="C112">
+        <v>36.2288</v>
+      </c>
+      <c r="D112">
+        <v>36.221200000000003</v>
+      </c>
+      <c r="E112">
+        <v>39.331099999999999</v>
+      </c>
+      <c r="F112">
+        <v>39.335000000000001</v>
+      </c>
+    </row>
+    <row r="144" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C144" t="s">
+        <v>26</v>
+      </c>
+      <c r="D144" t="s">
+        <v>28</v>
+      </c>
+      <c r="E144" t="s">
+        <v>27</v>
+      </c>
+      <c r="F144" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="145" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B145" t="s">
+        <v>19</v>
+      </c>
+      <c r="C145">
+        <v>94.54</v>
+      </c>
+      <c r="D145">
+        <v>93.23</v>
+      </c>
+      <c r="E145">
+        <v>95.04</v>
+      </c>
+      <c r="F145">
+        <v>91.95</v>
+      </c>
+    </row>
+    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B146" t="s">
+        <v>17</v>
+      </c>
+      <c r="C146">
+        <v>45.183100000000003</v>
+      </c>
+      <c r="D146">
+        <v>46.395699999999998</v>
+      </c>
+      <c r="E146">
+        <v>43.807899999999997</v>
+      </c>
+      <c r="F146">
+        <v>51.489899999999999</v>
+      </c>
+    </row>
+    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B147" t="s">
+        <v>18</v>
+      </c>
+      <c r="C147">
+        <v>70.218699999999998</v>
+      </c>
+      <c r="D147">
+        <v>79.430599999999998</v>
+      </c>
+      <c r="E147">
+        <v>68.185699999999997</v>
+      </c>
+      <c r="F147">
+        <v>84.784899999999993</v>
+      </c>
+    </row>
+    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B148" t="s">
+        <v>20</v>
+      </c>
+      <c r="C148">
+        <v>24.217500000000001</v>
+      </c>
+      <c r="D148">
+        <v>23.753299999999999</v>
+      </c>
+      <c r="E148">
+        <v>22.4284</v>
+      </c>
+      <c r="F148">
+        <v>27.597799999999999</v>
+      </c>
+    </row>
+    <row r="149" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B149" t="s">
+        <v>21</v>
+      </c>
+      <c r="C149">
+        <v>32.577199999999998</v>
+      </c>
+      <c r="D149">
+        <v>36.221200000000003</v>
+      </c>
+      <c r="E149">
+        <v>31.093399999999999</v>
+      </c>
+      <c r="F149">
+        <v>39.335000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>